<commit_message>
weer aan het report gewerkt
</commit_message>
<xml_diff>
--- a/src/Plaatje actions stateSpace representation.xlsx
+++ b/src/Plaatje actions stateSpace representation.xlsx
@@ -1,46 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="4240" yWindow="680" windowWidth="14060" windowHeight="12860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>HorizontalApproach(0),</t>
-  </si>
-  <si>
-    <t>HorizontalRetreat(1),</t>
-  </si>
-  <si>
-    <t>VerticalApproach(2),</t>
-  </si>
-  <si>
-    <t>VerticalRetreat(3),</t>
-  </si>
-  <si>
-    <t>Wait(4);</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,7 +142,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>409576</xdr:colOff>
+      <xdr:colOff>219076</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -159,9 +154,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="133350" y="114300"/>
-          <a:ext cx="5762626" cy="3619500"/>
+          <a:ext cx="6143626" cy="3378200"/>
           <a:chOff x="133350" y="114300"/>
-          <a:chExt cx="5762626" cy="3619500"/>
+          <a:chExt cx="5589314" cy="3619500"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -172,9 +167,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="133350" y="114300"/>
-            <a:ext cx="5762626" cy="3619500"/>
+            <a:ext cx="5589314" cy="3619500"/>
             <a:chOff x="133350" y="114300"/>
-            <a:chExt cx="5762626" cy="3619500"/>
+            <a:chExt cx="5589314" cy="3619500"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:grpSp>
@@ -185,9 +180,9 @@
           <xdr:grpSpPr>
             <a:xfrm>
               <a:off x="133350" y="114300"/>
-              <a:ext cx="5762626" cy="3619500"/>
+              <a:ext cx="5589314" cy="3619500"/>
               <a:chOff x="2466975" y="723900"/>
-              <a:chExt cx="5762626" cy="3619500"/>
+              <a:chExt cx="5589314" cy="3619500"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:grpSp>
@@ -198,9 +193,9 @@
             <xdr:grpSpPr>
               <a:xfrm>
                 <a:off x="2466975" y="723900"/>
-                <a:ext cx="5762626" cy="3609975"/>
+                <a:ext cx="5589314" cy="3609975"/>
                 <a:chOff x="2466975" y="723900"/>
-                <a:chExt cx="5762626" cy="3609975"/>
+                <a:chExt cx="5589314" cy="3609975"/>
               </a:xfrm>
             </xdr:grpSpPr>
             <xdr:sp macro="" textlink="">
@@ -1347,7 +1342,7 @@
               </xdr:nvSpPr>
               <xdr:spPr>
                 <a:xfrm>
-                  <a:off x="6877051" y="2190750"/>
+                  <a:off x="6703739" y="843643"/>
                   <a:ext cx="1352550" cy="1171575"/>
                 </a:xfrm>
                 <a:prstGeom prst="rect">
@@ -1464,7 +1459,7 @@
               </xdr:nvCxnSpPr>
               <xdr:spPr>
                 <a:xfrm flipH="1">
-                  <a:off x="6519862" y="2319337"/>
+                  <a:off x="6346550" y="972230"/>
                   <a:ext cx="304800" cy="0"/>
                 </a:xfrm>
                 <a:prstGeom prst="straightConnector1">
@@ -1499,7 +1494,7 @@
               </xdr:nvCxnSpPr>
               <xdr:spPr>
                 <a:xfrm rot="16200000" flipH="1" flipV="1">
-                  <a:off x="6672262" y="2357437"/>
+                  <a:off x="6498950" y="1010329"/>
                   <a:ext cx="0" cy="304800"/>
                 </a:xfrm>
                 <a:prstGeom prst="straightConnector1">
@@ -1534,7 +1529,7 @@
               </xdr:nvCxnSpPr>
               <xdr:spPr>
                 <a:xfrm flipH="1">
-                  <a:off x="6519862" y="2709862"/>
+                  <a:off x="6346550" y="1362755"/>
                   <a:ext cx="304800" cy="0"/>
                 </a:xfrm>
                 <a:prstGeom prst="straightConnector1">
@@ -1566,7 +1561,7 @@
               </xdr:nvCxnSpPr>
               <xdr:spPr>
                 <a:xfrm flipH="1">
-                  <a:off x="6519862" y="2890837"/>
+                  <a:off x="6346550" y="1543730"/>
                   <a:ext cx="304800" cy="0"/>
                 </a:xfrm>
                 <a:prstGeom prst="straightConnector1">
@@ -2122,7 +2117,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4257676" y="2466976"/>
+              <a:off x="4084364" y="1201512"/>
               <a:ext cx="190500" cy="190500"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
@@ -2487,42 +2482,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H18:H22"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2532,9 +2508,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2544,8 +2526,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>